<commit_message>
Sorting, Filtering, Text to Columns, Data Validation
</commit_message>
<xml_diff>
--- a/Excel/Data files/Lecture_6_Data.xlsx
+++ b/Excel/Data files/Lecture_6_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ds_30\Excel\Data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CD07FB-5C39-4542-8542-22848994BD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527E5722-00E6-4AF8-BC35-1EEFA4A61CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sorting" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
   <si>
     <t>Example</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>Fixed length</t>
-  </si>
-  <si>
-    <t>Student 8</t>
   </si>
   <si>
     <t>Student 9</t>
@@ -1458,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1533,16 +1530,16 @@
       <c r="F5" s="17"/>
       <c r="G5" s="3"/>
       <c r="H5" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I5" s="20">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="J5" s="20">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="K5" s="20">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1553,16 +1550,16 @@
         <v>27</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" s="20">
+        <v>99</v>
+      </c>
+      <c r="J6" s="20">
+        <v>83</v>
+      </c>
+      <c r="K6" s="20">
         <v>85</v>
-      </c>
-      <c r="J6" s="20">
-        <v>53</v>
-      </c>
-      <c r="K6" s="20">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1593,16 +1590,16 @@
         <v>24</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="20">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="J8" s="20">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="K8" s="20">
-        <v>85</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1613,16 +1610,16 @@
         <v>25</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I9" s="20">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="J9" s="20">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="K9" s="20">
-        <v>82</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1708,8 +1705,8 @@
       <c r="B19" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H13:I18">
-    <sortCondition ref="H13:H18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H5:K9">
+    <sortCondition descending="1" ref="I5:I9"/>
   </sortState>
   <mergeCells count="6">
     <mergeCell ref="T1:U1"/>
@@ -1726,11 +1723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1837,7 +1833,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="20.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="34">
         <v>1</v>
       </c>
@@ -1933,7 +1929,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="20.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="36">
         <v>4</v>
       </c>
@@ -1992,15 +1988,7 @@
       <c r="B18" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="H4:N9" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="100"/>
-        <filter val="85"/>
-        <filter val="99"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="H4:N9" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="6">
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="G1:J1"/>
@@ -2018,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2114,7 +2102,7 @@
         <v>85</v>
       </c>
       <c r="L5" s="21">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O5" s="33" t="s">
         <v>3</v>
@@ -2139,7 +2127,9 @@
       <c r="K6" s="21">
         <v>43</v>
       </c>
-      <c r="L6" s="21"/>
+      <c r="L6" s="21">
+        <v>99</v>
+      </c>
       <c r="O6" s="33" t="s">
         <v>4</v>
       </c>
@@ -2163,7 +2153,9 @@
       <c r="K7" s="21">
         <v>79</v>
       </c>
-      <c r="L7" s="21"/>
+      <c r="L7" s="21">
+        <v>87</v>
+      </c>
       <c r="O7" s="33" t="s">
         <v>10</v>
       </c>
@@ -2226,9 +2218,7 @@
       <c r="H10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="21">
-        <v>0</v>
-      </c>
+      <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
@@ -2271,7 +2261,7 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L9" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
@@ -2279,12 +2269,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>$O$4:$O$10</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>10</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error in data entry" error="Please enter score between 0 and 100" promptTitle="Input rules" prompt="Score should be less than 100" sqref="I10" xr:uid="{00000000-0002-0000-0200-000003000000}">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2296,7 +2282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2459,13 +2447,13 @@
         <v>11</v>
       </c>
       <c r="I10" s="21">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J10" s="21">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="K10" s="21">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -2474,43 +2462,35 @@
         <v>12</v>
       </c>
       <c r="I11" s="21">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="J11" s="21">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="K11" s="21">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" s="25"/>
-      <c r="H12" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="21">
-        <v>45</v>
-      </c>
-      <c r="J12" s="21">
-        <v>63</v>
-      </c>
-      <c r="K12" s="21">
-        <v>72</v>
-      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D13" s="25"/>
       <c r="H13" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="21">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="J13" s="21">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K13" s="21">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -2541,7 +2521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2600,7 +2582,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>2</v>
@@ -2621,7 +2603,7 @@
         <v>5</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J5" s="21">
         <v>99</v>
@@ -2638,13 +2620,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6" s="21">
         <v>100</v>
@@ -2661,13 +2643,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="21" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J7" s="21">
         <v>85</v>
@@ -2686,7 +2668,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" s="21">
         <v>55</v>
@@ -2705,7 +2687,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" s="21">
         <v>65</v>

</xml_diff>